<commit_message>
23/04/04 C조 팀프 회의
</commit_message>
<xml_diff>
--- a/일정표 수정본.xlsx
+++ b/일정표 수정본.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Atents\TeamProject\other\AtentsTeamCProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B04D99-EA46-43CC-8893-2E9BAC61E2AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01962AC-40DF-4982-B4C1-ECD68CE5BD98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="67">
   <si>
     <t>황준호</t>
   </si>
@@ -179,40 +179,62 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>작업물 확인 불가</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>스크립트 오류, 프리팹 확인 불가</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>팀 퇴출</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">필드 맵 구현 (일반 필드맵 1~2개이상, 보스방 1개(바위골렘용으로)) </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4주차 04/03</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>5주차 04/10</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>6주차 04/17</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>중간평가</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">필드 맵 구현 (일반 필드맵 1~2개이상, 보스방 1개(바위골렘용으로)) </t>
+  </si>
+  <si>
+    <t>원거리 몬스터 구현</t>
+  </si>
+  <si>
+    <t>파이어볼 딜레이 없이 발사중. 수정필요</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>맵에 함정이나 오브젝트가 일체 없음. 추후 배치 필요</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 원거리 몬스터 파이어볼 구현 2. 보스몬스터 구현</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">플레이어 애니메이션 블랜딩, 무기 변경 구현, 표지판(설명용) </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>여유</t>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>작업물 확인 불가</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>스크립트 오류, 프리팹 확인 불가</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>팀 퇴출</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">필드 맵 구현 (일반 필드맵 1~2개이상, 보스방 1개(바위골렘용으로)) </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>4주차 04/03</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>5주차 04/10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>6주차 04/17</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>중간평가</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -249,7 +271,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -343,6 +365,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -361,7 +395,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -443,22 +477,37 @@
     <xf numFmtId="9" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -969,8 +1018,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="T20" sqref="T20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1046,10 +1095,10 @@
       </c>
       <c r="F3" s="29"/>
       <c r="G3" s="29"/>
-      <c r="H3" s="30" t="s">
+      <c r="H3" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="30"/>
+      <c r="I3" s="28"/>
       <c r="N3" t="s">
         <v>23</v>
       </c>
@@ -1064,11 +1113,11 @@
       <c r="D4" s="15">
         <v>0.3</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
       <c r="H4" s="2" t="s">
         <v>44</v>
       </c>
@@ -1088,10 +1137,10 @@
       <c r="E5" s="29"/>
       <c r="F5" s="29"/>
       <c r="G5" s="29"/>
-      <c r="H5" s="30" t="s">
+      <c r="H5" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="30"/>
+      <c r="I5" s="28"/>
       <c r="N5" t="s">
         <v>47</v>
       </c>
@@ -1103,11 +1152,11 @@
       <c r="D6" s="17">
         <v>0.8</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1121,10 +1170,10 @@
       <c r="E7" s="29"/>
       <c r="F7" s="29"/>
       <c r="G7" s="29"/>
-      <c r="H7" s="30" t="s">
+      <c r="H7" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="30"/>
+      <c r="I7" s="28"/>
       <c r="N7" t="s">
         <v>39</v>
       </c>
@@ -1136,11 +1185,11 @@
       <c r="D8" s="26">
         <v>0</v>
       </c>
-      <c r="E8" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
+      <c r="E8" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -1182,10 +1231,10 @@
       <c r="E10" s="29"/>
       <c r="F10" s="29"/>
       <c r="G10" s="29"/>
-      <c r="H10" s="30" t="s">
+      <c r="H10" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="30"/>
+      <c r="I10" s="28"/>
       <c r="N10" t="s">
         <v>24</v>
       </c>
@@ -1200,11 +1249,11 @@
       <c r="D11" s="15">
         <v>0</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -1218,10 +1267,10 @@
       <c r="E12" s="29"/>
       <c r="F12" s="29"/>
       <c r="G12" s="29"/>
-      <c r="H12" s="30" t="s">
+      <c r="H12" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="30"/>
+      <c r="I12" s="28"/>
       <c r="N12" t="s">
         <v>40</v>
       </c>
@@ -1230,9 +1279,9 @@
       <c r="C13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -1248,10 +1297,10 @@
         <v>38</v>
       </c>
       <c r="G14" s="29"/>
-      <c r="H14" s="30" t="s">
+      <c r="H14" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="30"/>
+      <c r="I14" s="28"/>
       <c r="M14" t="s">
         <v>34</v>
       </c>
@@ -1266,11 +1315,11 @@
       <c r="D15" s="26">
         <v>0</v>
       </c>
-      <c r="E15" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
+      <c r="E15" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
       <c r="N15" t="s">
         <v>48</v>
       </c>
@@ -1323,15 +1372,15 @@
       <c r="D17" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="30" t="s">
+      <c r="E17" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="30"/>
+      <c r="I17" s="28"/>
       <c r="N17" t="s">
         <v>21</v>
       </c>
@@ -1346,6 +1395,12 @@
       <c r="C18" s="25">
         <v>1</v>
       </c>
+      <c r="D18" s="33">
+        <v>0.75</v>
+      </c>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
       <c r="N18" t="s">
         <v>32</v>
       </c>
@@ -1362,15 +1417,15 @@
         <v>30</v>
       </c>
       <c r="D19" s="29"/>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="30" t="s">
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I19" s="30"/>
+      <c r="I19" s="28"/>
       <c r="N19" t="s">
         <v>41</v>
       </c>
@@ -1382,6 +1437,9 @@
       <c r="C20" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="D20" s="33">
+        <v>0.75</v>
+      </c>
       <c r="N20" t="s">
         <v>22</v>
       </c>
@@ -1398,13 +1456,11 @@
         <v>38</v>
       </c>
       <c r="D21" s="29"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="I21" s="30"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
       <c r="N21" t="s">
         <v>28</v>
       </c>
@@ -1419,15 +1475,15 @@
       <c r="D22" s="26">
         <v>0</v>
       </c>
-      <c r="E22" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
+      <c r="E22" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C23" s="1">
         <v>45012</v>
@@ -1458,17 +1514,19 @@
       <c r="B24" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="32"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="30" t="s">
+      <c r="C24" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="31"/>
+      <c r="E24" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I24" s="30"/>
+      <c r="I24" s="28"/>
       <c r="M24" t="s">
         <v>1</v>
       </c>
@@ -1480,8 +1538,11 @@
       <c r="B25" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>10</v>
+      <c r="C25" s="33">
+        <v>0.8</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>63</v>
       </c>
       <c r="M25" t="s">
         <v>2</v>
@@ -1492,24 +1553,29 @@
         <v>6</v>
       </c>
       <c r="B26" s="3"/>
-      <c r="C26" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="D26" s="32"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="30" t="s">
+      <c r="C26" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="31"/>
+      <c r="E26" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I26" s="30"/>
+      <c r="I26" s="28"/>
       <c r="M26" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="C27" s="2" t="s">
-        <v>10</v>
+      <c r="C27" s="33">
+        <v>0.75</v>
+      </c>
+      <c r="D27" s="24" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
@@ -1520,7 +1586,7 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C29" s="1">
         <v>45012</v>
@@ -1557,15 +1623,17 @@
       <c r="B30" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="30" t="s">
+      <c r="C30" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="29"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I30" s="30"/>
+      <c r="I30" s="28"/>
       <c r="O30" s="22"/>
       <c r="P30" s="22"/>
       <c r="Q30" s="22"/>
@@ -1584,15 +1652,17 @@
         <v>6</v>
       </c>
       <c r="B32" s="3"/>
-      <c r="C32" s="29"/>
+      <c r="C32" s="37" t="s">
+        <v>66</v>
+      </c>
       <c r="D32" s="29"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="30" t="s">
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I32" s="30"/>
+      <c r="I32" s="28"/>
       <c r="M32" s="22"/>
       <c r="N32" s="22"/>
       <c r="O32" s="23"/>
@@ -1607,7 +1677,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="1">
@@ -1617,46 +1687,22 @@
       <c r="N34" s="23"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D35" s="28" t="s">
-        <v>60</v>
+      <c r="D35" s="27" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D36" s="28"/>
+      <c r="D36" s="27"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D37" s="28"/>
+      <c r="D37" s="27"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D38" s="28"/>
+      <c r="D38" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="D35:D38"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F14:G14"/>
+  <mergeCells count="42">
+    <mergeCell ref="C30:D30"/>
     <mergeCell ref="E8:G8"/>
     <mergeCell ref="E22:G22"/>
     <mergeCell ref="C32:D32"/>
@@ -1673,6 +1719,31 @@
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="E17:G17"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="D35:D38"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="E6:G6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>

</xml_diff>

<commit_message>
23/04/06 C조 팀프 회의
골렘 패키지 추가됨
</commit_message>
<xml_diff>
--- a/일정표 수정본.xlsx
+++ b/일정표 수정본.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Atents\TeamProject\other\AtentsTeamCProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E26D4F8-D695-4178-8E29-A59D64E2D59F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196B0D55-2DBD-47B7-8C35-82DDAF2FF99A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="68">
   <si>
     <t>황준호</t>
   </si>
@@ -217,23 +217,26 @@
     <t>원거리 몬스터 구현</t>
   </si>
   <si>
-    <t>파이어볼 딜레이 없이 발사중. 수정필요</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>맵에 함정이나 오브젝트가 일체 없음. 추후 배치 필요</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">플레이어 애니메이션 블랜딩, 무기 변경 구현, 표지판(설명용) </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>여유</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>보스몬스터 구현</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>파이어볼 딜레이 없이 발사중. 수정 완</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어 애니메이션 블렌딩 구현 성공</t>
+  </si>
+  <si>
+    <t xml:space="preserve">플레이어 애니메이션 블랜딩, 게임 UI 구현, 표지판(설명용) </t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -395,7 +398,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -480,35 +483,32 @@
     <xf numFmtId="9" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1019,7 +1019,7 @@
   <dimension ref="A1:S38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="Q28" sqref="Q28"/>
+      <selection activeCell="E26" sqref="E26:G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1095,10 +1095,10 @@
       </c>
       <c r="F3" s="29"/>
       <c r="G3" s="29"/>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="32"/>
+      <c r="I3" s="28"/>
       <c r="N3" t="s">
         <v>23</v>
       </c>
@@ -1113,11 +1113,11 @@
       <c r="D4" s="15">
         <v>0.3</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
       <c r="H4" s="2" t="s">
         <v>44</v>
       </c>
@@ -1137,10 +1137,10 @@
       <c r="E5" s="29"/>
       <c r="F5" s="29"/>
       <c r="G5" s="29"/>
-      <c r="H5" s="32" t="s">
+      <c r="H5" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="32"/>
+      <c r="I5" s="28"/>
       <c r="N5" t="s">
         <v>47</v>
       </c>
@@ -1152,11 +1152,11 @@
       <c r="D6" s="17">
         <v>0.8</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1170,10 +1170,10 @@
       <c r="E7" s="29"/>
       <c r="F7" s="29"/>
       <c r="G7" s="29"/>
-      <c r="H7" s="32" t="s">
+      <c r="H7" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="32"/>
+      <c r="I7" s="28"/>
       <c r="N7" t="s">
         <v>39</v>
       </c>
@@ -1185,11 +1185,11 @@
       <c r="D8" s="26">
         <v>0</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -1231,10 +1231,10 @@
       <c r="E10" s="29"/>
       <c r="F10" s="29"/>
       <c r="G10" s="29"/>
-      <c r="H10" s="32" t="s">
+      <c r="H10" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="32"/>
+      <c r="I10" s="28"/>
       <c r="N10" t="s">
         <v>24</v>
       </c>
@@ -1249,11 +1249,11 @@
       <c r="D11" s="15">
         <v>0</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="E11" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -1267,10 +1267,10 @@
       <c r="E12" s="29"/>
       <c r="F12" s="29"/>
       <c r="G12" s="29"/>
-      <c r="H12" s="32" t="s">
+      <c r="H12" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="32"/>
+      <c r="I12" s="28"/>
       <c r="N12" t="s">
         <v>40</v>
       </c>
@@ -1279,9 +1279,9 @@
       <c r="C13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -1297,10 +1297,10 @@
         <v>38</v>
       </c>
       <c r="G14" s="29"/>
-      <c r="H14" s="32" t="s">
+      <c r="H14" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="32"/>
+      <c r="I14" s="28"/>
       <c r="M14" t="s">
         <v>34</v>
       </c>
@@ -1315,11 +1315,11 @@
       <c r="D15" s="26">
         <v>0</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
       <c r="N15" t="s">
         <v>48</v>
       </c>
@@ -1377,10 +1377,10 @@
       </c>
       <c r="F17" s="36"/>
       <c r="G17" s="36"/>
-      <c r="H17" s="32" t="s">
+      <c r="H17" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="32"/>
+      <c r="I17" s="28"/>
       <c r="N17" t="s">
         <v>21</v>
       </c>
@@ -1398,9 +1398,9 @@
       <c r="D18" s="27">
         <v>0.75</v>
       </c>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
       <c r="N18" t="s">
         <v>32</v>
       </c>
@@ -1422,10 +1422,10 @@
       </c>
       <c r="F19" s="36"/>
       <c r="G19" s="36"/>
-      <c r="H19" s="32" t="s">
+      <c r="H19" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I19" s="32"/>
+      <c r="I19" s="28"/>
       <c r="N19" t="s">
         <v>41</v>
       </c>
@@ -1456,9 +1456,9 @@
         <v>38</v>
       </c>
       <c r="D21" s="29"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
       <c r="N21" t="s">
         <v>28</v>
       </c>
@@ -1473,11 +1473,11 @@
       <c r="D22" s="26">
         <v>0</v>
       </c>
-      <c r="E22" s="30" t="s">
+      <c r="E22" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
@@ -1516,15 +1516,15 @@
         <v>60</v>
       </c>
       <c r="D24" s="36"/>
-      <c r="E24" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="32" t="s">
+      <c r="E24" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I24" s="32"/>
+      <c r="I24" s="28"/>
       <c r="M24" t="s">
         <v>1</v>
       </c>
@@ -1540,7 +1540,10 @@
         <v>0.8</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="E25" t="s">
+        <v>66</v>
       </c>
       <c r="M25" t="s">
         <v>2</v>
@@ -1555,15 +1558,15 @@
         <v>61</v>
       </c>
       <c r="D26" s="36"/>
-      <c r="E26" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="32" t="s">
+      <c r="E26" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I26" s="32"/>
+      <c r="I26" s="28"/>
       <c r="M26" t="s">
         <v>3</v>
       </c>
@@ -1573,7 +1576,7 @@
         <v>0.75</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
@@ -1621,19 +1624,17 @@
       <c r="B30" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="28" t="s">
-        <v>65</v>
+      <c r="C30" s="34" t="s">
+        <v>63</v>
       </c>
       <c r="D30" s="29"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="31" t="s">
+      <c r="G30" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="H30" s="32" t="s">
+      <c r="H30" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I30" s="32"/>
+      <c r="I30" s="28"/>
       <c r="O30" s="22"/>
       <c r="P30" s="22"/>
       <c r="Q30" s="22"/>
@@ -1646,24 +1647,22 @@
       <c r="C31" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G31" s="31"/>
+      <c r="G31" s="30"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>6</v>
       </c>
       <c r="B32" s="3"/>
-      <c r="C32" s="28" t="s">
-        <v>65</v>
+      <c r="C32" s="34" t="s">
+        <v>63</v>
       </c>
       <c r="D32" s="29"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="37"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="32" t="s">
+      <c r="G32" s="30"/>
+      <c r="H32" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I32" s="32"/>
+      <c r="I32" s="28"/>
       <c r="M32" s="22"/>
       <c r="N32" s="22"/>
       <c r="O32" s="23"/>
@@ -1675,7 +1674,7 @@
       <c r="C33" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G33" s="31"/>
+      <c r="G33" s="30"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="24" t="s">
@@ -1689,21 +1688,46 @@
       <c r="N34" s="23"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D35" s="31" t="s">
+      <c r="D35" s="30" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D36" s="31"/>
+      <c r="D36" s="30"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D37" s="31"/>
+      <c r="D37" s="30"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D38" s="31"/>
+      <c r="D38" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="D35:D38"/>
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="C30:D30"/>
     <mergeCell ref="H17:I17"/>
     <mergeCell ref="H19:I19"/>
     <mergeCell ref="C3:D3"/>
@@ -1720,31 +1744,6 @@
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="D35:D38"/>
-    <mergeCell ref="G30:G33"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E13:G13"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>

</xml_diff>